<commit_message>
adding comparison QCs to the driver and config checking
</commit_message>
<xml_diff>
--- a/paqc/data/Status_QC.xlsx
+++ b/paqc/data/Status_QC.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18828"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7221D94A-A9C1-46A0-9FE3-E0BA899DC3A7}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C879E2D-BE07-49EC-A173-3854EDD0C8C4}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -38,7 +38,7 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>All</t>
+    <t>General</t>
   </si>
   <si>
     <t>Testing if all column names of dataframe have no special characters and no
@@ -61,9 +61,6 @@
     <t>Not needed anymore, happens at read in of data.</t>
   </si>
   <si>
-    <t xml:space="preserve">All </t>
-  </si>
-  <si>
     <t>All columns ending in FLAG, COUNT or FREQ should be 0 or positive, and never missing. </t>
   </si>
   <si>
@@ -110,7 +107,7 @@
 date and first exposure date are on different days.</t>
   </si>
   <si>
-    <t>Get rid of it?</t>
+    <t>SLIGHTLY ALTERED: Checks that when first exposure date is before last exposure date, the count for that feature is bigger than 1.</t>
   </si>
   <si>
     <t>No missing patient IDs</t>
@@ -184,7 +181,7 @@
 90 days different. </t>
   </si>
   <si>
-    <t xml:space="preserve">Every patient in CN01 should meet the stratification criteria, CC01_CS. </t>
+    <t>Every patient in CN01 should meet the stratification criteria, CC01_CS. </t>
   </si>
   <si>
     <t>no CC01_CS criteria yet</t>
@@ -209,12 +206,6 @@
     <t>CS04</t>
   </si>
   <si>
-    <t xml:space="preserve">Dataset has NO patients in it who meet at least one of the selection criteria listed in CC01_CP </t>
-  </si>
-  <si>
-    <t>relevant columns are not kept in this dataset</t>
-  </si>
-  <si>
     <t>Flag proportions table</t>
   </si>
   <si>
@@ -226,6 +217,9 @@
   </si>
   <si>
     <t>Every row should have a unique description. There should be no duplicate descriptions</t>
+  </si>
+  <si>
+    <t>Compare</t>
   </si>
   <si>
     <t>Two dataframes have the same columns and they are in the same order.
@@ -322,13 +316,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,13 +339,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -365,18 +358,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,18 +674,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEDF6A8D-1A12-48F1-9316-F02087B8D189}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{A30CB92B-A4F5-5BD0-BB60-1F08E341DEA8}">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0" xr3:uid="{A30CB92B-A4F5-5BD0-BB60-1F08E341DEA8}">
+      <selection activeCell="B40" sqref="B40:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="80.7109375" customWidth="1"/>
-    <col min="7" max="7" width="55.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="77.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="70" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -734,19 +728,19 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="4"/>
       <c r="G3" t="s">
         <v>13</v>
       </c>
@@ -755,11 +749,11 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -767,7 +761,7 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
@@ -777,51 +771,51 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="30">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="30">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -829,10 +823,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -840,25 +834,25 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5"/>
+      <c r="E9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="45">
       <c r="A10">
@@ -868,7 +862,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -876,7 +870,7 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11">
@@ -886,7 +880,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -894,7 +888,7 @@
       <c r="E11" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="45">
       <c r="A12">
@@ -904,7 +898,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -912,9 +906,9 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="60">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="120">
       <c r="A13">
         <v>12</v>
       </c>
@@ -922,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -930,27 +924,27 @@
       <c r="E13" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="45">
-      <c r="A14" s="14">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="75">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -961,15 +955,15 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
@@ -979,15 +973,15 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17">
@@ -997,15 +991,15 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18">
@@ -1014,8 +1008,8 @@
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>34</v>
+      <c r="C18" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -1023,7 +1017,7 @@
       <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
@@ -1032,8 +1026,8 @@
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>35</v>
+      <c r="C19" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1041,7 +1035,7 @@
       <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20">
@@ -1050,16 +1044,16 @@
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>36</v>
+      <c r="C20" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="30">
       <c r="A21">
@@ -1068,10 +1062,10 @@
       <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="4"/>
+      <c r="C21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:7" ht="45">
       <c r="A22">
@@ -1080,21 +1074,35 @@
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="C23" s="12"/>
-      <c r="F23" s="7"/>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
         <v>40</v>
@@ -1105,334 +1113,328 @@
       <c r="E24" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="60">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" ht="30">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="7"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>45</v>
       </c>
-      <c r="D28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" t="s">
-        <v>47</v>
+      <c r="C29" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="60">
       <c r="A30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s">
         <v>50</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>46</v>
-      </c>
-      <c r="C32" t="s">
         <v>51</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="2" t="s">
+    </row>
+    <row r="32" spans="1:7" ht="45">
+      <c r="A32" s="12">
+        <v>31</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="30">
-      <c r="A33" s="14">
-        <v>31</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="4"/>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
         <v>54</v>
       </c>
-      <c r="C34" t="s">
+      <c r="F34" s="3"/>
+      <c r="G34" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>57</v>
       </c>
       <c r="C35" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F36" s="4"/>
-      <c r="G36" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="45">
       <c r="A37">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>58</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="2" t="s">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="F43" s="7"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="45">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" ht="30">
+      <c r="A40">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" ht="30">
+      <c r="A41">
+        <v>47</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:7" ht="30">
+      <c r="A42">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:7" ht="90">
+      <c r="A43">
+        <v>49</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:7" ht="30">
       <c r="A44">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" ht="45">
+      <c r="A45">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45">
-        <v>41</v>
-      </c>
-      <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" t="s">
-        <v>63</v>
-      </c>
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46">
-        <v>42</v>
-      </c>
-      <c r="B46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>64</v>
-      </c>
-      <c r="F46" s="4"/>
-    </row>
-    <row r="49" spans="1:6" ht="30">
-      <c r="A49">
-        <v>46</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" ht="30">
-      <c r="A50">
-        <v>47</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E50" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="1:6" ht="30">
-      <c r="A51">
-        <v>48</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:6" ht="90">
-      <c r="A52">
-        <v>49</v>
-      </c>
-      <c r="C52" s="10" t="s">
+      <c r="C45" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E52" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="1:6" ht="30">
-      <c r="A53">
-        <v>50</v>
-      </c>
-      <c r="C53" s="1" t="s">
+    </row>
+    <row r="46" spans="1:7" ht="45">
+      <c r="C46" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E53" t="s">
-        <v>10</v>
-      </c>
-      <c r="F53" s="5"/>
-    </row>
-    <row r="54" spans="1:6" ht="45">
-      <c r="A54">
-        <v>52</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="45">
-      <c r="C55" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="93.75" customHeight="1">
-      <c r="C56" s="1"/>
+    </row>
+    <row r="47" spans="1:7" ht="93.75" customHeight="1">
+      <c r="C47" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:G52">
-    <sortCondition ref="A2:A52"/>
+  <sortState ref="A2:G43">
+    <sortCondition ref="A2:A43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>